<commit_message>
Editar Dados Cadastrais para correção
</commit_message>
<xml_diff>
--- a/bos/Pendências de Validação.xlsx
+++ b/bos/Pendências de Validação.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="167">
   <si>
     <t>Campo</t>
   </si>
@@ -507,10 +507,34 @@
     <t>diminuir campo</t>
   </si>
   <si>
-    <t>Tela ESCOLARIDADE</t>
-  </si>
-  <si>
-    <t>Tela Proficiência</t>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>Corrigir insere linhas (iniciar na linha 1)</t>
+  </si>
+  <si>
+    <t>Remover campo Idioma X ao clicar em [+]</t>
+  </si>
+  <si>
+    <t>Incluir [-] em Novo Idioma/Instiruição para remover campo</t>
+  </si>
+  <si>
+    <t>Corrigir largura do campo "Escreve"</t>
+  </si>
+  <si>
+    <t>Exibir "Órgão financiador" se "Bolsa?" = sim</t>
+  </si>
+  <si>
+    <t>Incluir botão [+] em "Órgão Financiador"</t>
+  </si>
+  <si>
+    <t>Inclruir botão [-] em Novo Órgão para remover campo</t>
+  </si>
+  <si>
+    <t>UF Nascimento</t>
+  </si>
+  <si>
+    <t>Aparece se Nacionalidade = Brasil</t>
   </si>
 </sst>
 </file>
@@ -883,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E80"/>
+  <dimension ref="A2:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,10 +1634,51 @@
       <c r="B79" t="s">
         <v>157</v>
       </c>
+      <c r="C79" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>158</v>
+      <c r="C80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>165</v>
+      </c>
+      <c r="C87" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>